<commit_message>
CORRECCION 08 -faltantes: bonader y diaz johard
</commit_message>
<xml_diff>
--- a/Desafios/08/Pair Programming.xlsx
+++ b/Desafios/08/Pair Programming.xlsx
@@ -242,8 +242,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -456,8 +456,8 @@
   </sheetPr>
   <dimension ref="B4:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -654,7 +654,7 @@
       <c r="B21" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="6" t="s">

</xml_diff>